<commit_message>
modificando la h de horas a MTTR
</commit_message>
<xml_diff>
--- a/Tabla4_IEEE.xlsx
+++ b/Tabla4_IEEE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\milla\Documents\Maestria (Tesis)\Capitulo 2\Programa_para_modelo _optimizacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6944434F-29A8-4698-9C0A-A481B8383924}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{806DBB6B-C2F4-4680-978E-3252A66E53C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5760" yWindow="0" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,9 +39,6 @@
     <t>MTTF(horas)</t>
   </si>
   <si>
-    <t>MTTR(Horas)</t>
-  </si>
-  <si>
     <t>Mantenimiento de semanas por año</t>
   </si>
   <si>
@@ -85,6 +82,9 @@
   </si>
   <si>
     <t>Nuclear</t>
+  </si>
+  <si>
+    <t>MTTR(horas)</t>
   </si>
 </sst>
 </file>
@@ -405,12 +405,15 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="30.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.6640625" customWidth="1"/>
+    <col min="6" max="6" width="31.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -427,21 +430,21 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2">
         <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2">
         <v>2940</v>
@@ -455,13 +458,13 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3">
         <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D3">
         <v>450</v>
@@ -475,13 +478,13 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4">
         <v>50</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4">
         <v>1980</v>
@@ -495,13 +498,13 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5">
         <v>76</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5">
         <v>1960</v>
@@ -515,13 +518,13 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6">
         <v>100</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D6">
         <v>1200</v>
@@ -535,13 +538,13 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7">
         <v>155</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D7">
         <v>960</v>
@@ -555,13 +558,13 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8">
         <v>197</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D8">
         <v>950</v>
@@ -575,13 +578,13 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9">
         <v>350</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D9">
         <v>1150</v>
@@ -595,13 +598,13 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10">
         <v>400</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D10">
         <v>1100</v>

</xml_diff>